<commit_message>
Updated the Extent Reports.
</commit_message>
<xml_diff>
--- a/target/classes/com/bryne/qa/testdata/BryneTestData.xlsx
+++ b/target/classes/com/bryne/qa/testdata/BryneTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek\eclipse-workspace\bryneMicrositeTest\src\main\java\com\bryne\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>First name</t>
   </si>
@@ -57,39 +57,15 @@
   </si>
   <si>
     <t>Karnatka</t>
-  </si>
-  <si>
-    <t>Rom</t>
-  </si>
-  <si>
-    <t>Kom</t>
-  </si>
-  <si>
-    <t>Bmumbai</t>
-  </si>
-  <si>
-    <t>Maharastraa</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>Aakhri</t>
-  </si>
-  <si>
-    <t>Pasta</t>
-  </si>
-  <si>
-    <t>Varanasi</t>
-  </si>
-  <si>
-    <t>UP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,14 +381,14 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
@@ -425,7 +402,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -448,7 +425,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>900000003</v>
       </c>
       <c r="D2" t="s">
@@ -466,51 +443,52 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>9000000215</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>900000003</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>40001</v>
+        <v>300023</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>90000004</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>900000003</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>231218</v>
+        <v>300023</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>